<commit_message>
Design du P.L JOB SHOP Machine multiples !
</commit_message>
<xml_diff>
--- a/26. Recherche opérationnelle en Excel/33 - MULTIPLES - JOB SHOP SUR 2 MACHINES ET VOYAGEUR DE COMMERCE/Deal-with-Sequencing-Problems-using-Excel-Solver.xlsx
+++ b/26. Recherche opérationnelle en Excel/33 - MULTIPLES - JOB SHOP SUR 2 MACHINES ET VOYAGEUR DE COMMERCE/Deal-with-Sequencing-Problems-using-Excel-Solver.xlsx
@@ -5,111 +5,111 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\python-data-science2\26. Recherche opérationnelle en Excel\33 - MULTIPLES - JOB SHOP ET VOYAGEUR DE COMMERCE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\python-data-science2\26. Recherche opérationnelle en Excel\33 - MULTIPLES - JOB SHOP SUR 2 MACHINES ET VOYAGEUR DE COMMERCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="72" windowWidth="20112" windowHeight="7992" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="72" windowWidth="20112" windowHeight="7992"/>
   </bookViews>
   <sheets>
-    <sheet name="Index Function" sheetId="3" r:id="rId1"/>
-    <sheet name="Case 1" sheetId="1" r:id="rId2"/>
-    <sheet name="Case 2" sheetId="2" r:id="rId3"/>
+    <sheet name="JOB SHOP MACHINES MULTIPLES" sheetId="2" r:id="rId1"/>
+    <sheet name="Index Function" sheetId="3" r:id="rId2"/>
+    <sheet name="Case 1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'Case 1'!$P$3:$P$13</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">'Case 2'!$G$3:$G$8</definedName>
-    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Case 1'!$P$3:$P$13</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'JOB SHOP MACHINES MULTIPLES'!$G$3:$G$8</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">100</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Case 1'!$P$3:$P$13</definedName>
-    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Case 2'!$G$3:$G$8</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Case 1'!$P$3:$P$13</definedName>
-    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Case 2'!$G$3:$G$8</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Case 1'!$P$3:$P$13</definedName>
-    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Case 2'!$G$3:$G$8</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Case 1'!$P$3:$P$13</definedName>
-    <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Case 2'!$G$3:$G$8</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Case 1'!$P$3:$P$13</definedName>
-    <definedName name="solver_lhs5" localSheetId="2" hidden="1">'Case 2'!$I$3:$I$8</definedName>
-    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Case 1'!$P$3:$P$13</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'JOB SHOP MACHINES MULTIPLES'!$G$3:$G$8</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Case 1'!$P$3:$P$13</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'JOB SHOP MACHINES MULTIPLES'!$G$3:$G$8</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Case 1'!$P$3:$P$13</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'JOB SHOP MACHINES MULTIPLES'!$G$3:$G$8</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Case 1'!$P$3:$P$13</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'JOB SHOP MACHINES MULTIPLES'!$G$3:$G$8</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">'Case 1'!$P$3:$P$13</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'JOB SHOP MACHINES MULTIPLES'!$I$3:$I$8</definedName>
     <definedName name="solver_lin" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">4</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">5</definedName>
-    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'Case 1'!$Q$14</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">'Case 2'!$G$9</definedName>
-    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Case 1'!$Q$14</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'JOB SHOP MACHINES MULTIPLES'!$G$9</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="1" hidden="1">6</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">6</definedName>
-    <definedName name="solver_rel3" localSheetId="1" hidden="1">4</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">6</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">4</definedName>
-    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_rel5" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel5" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">11</definedName>
-    <definedName name="solver_rhs1" localSheetId="2" hidden="1">6</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">AllDifferent</definedName>
-    <definedName name="solver_rhs2" localSheetId="2" hidden="1">"AllDifferent"</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">integer</definedName>
-    <definedName name="solver_rhs3" localSheetId="2" hidden="1">"integer"</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">11</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">6</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">AllDifferent</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">"AllDifferent"</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">integer</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">"integer"</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_rhs5" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rhs5" localSheetId="2" hidden="1">'Case 2'!$K$3:$K$8</definedName>
-    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">'JOB SHOP MACHINES MULTIPLES'!$K$3:$K$8</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">100</definedName>
-    <definedName name="solver_tol" localSheetId="1" hidden="1">0.05</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.05</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.05</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>Boston</t>
   </si>
@@ -157,12 +157,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Due date</t>
-  </si>
-  <si>
-    <t>Days needed</t>
   </si>
   <si>
     <t>Job</t>
@@ -182,12 +176,6 @@
 2</t>
   </si>
   <si>
-    <t>Total Days</t>
-  </si>
-  <si>
-    <t>Due Date</t>
-  </si>
-  <si>
     <t>&lt;=</t>
   </si>
   <si>
@@ -208,9 +196,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Les variables de décision</t>
-  </si>
-  <si>
     <t>La durée totale qu'on veut minimiser (function objectif)</t>
   </si>
   <si>
@@ -223,9 +208,6 @@
     <t>machine 1</t>
   </si>
   <si>
-    <t>Solveur result</t>
-  </si>
-  <si>
     <t>JOB 2</t>
   </si>
   <si>
@@ -247,10 +229,55 @@
     <t>JOB 5</t>
   </si>
   <si>
-    <t>JOB SHOP !!!</t>
-  </si>
-  <si>
     <t>Note : On voit que le solveur dispatche les jobs (tâches) sur les machines , en tenant compte de la date maximum de délivrance du job , et qu'il arrive à minimiser la date totale du projet !</t>
+  </si>
+  <si>
+    <t>makespan</t>
+  </si>
+  <si>
+    <t>fin du projet'</t>
+  </si>
+  <si>
+    <t>Les variables de décision, elles se modifient en fonction du résultat final trouvé par le solveur</t>
+  </si>
+  <si>
+    <t>Durée</t>
+  </si>
+  <si>
+    <t>Date butoir</t>
+  </si>
+  <si>
+    <t>Durée totale en jours</t>
+  </si>
+  <si>
+    <t>JOB SHOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infos de base de mon projet : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dispatch des tâches effectuées par le solveur linéaire : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On trace le résultat du solveur à la main sous forme de GANTT pour mieux comprendre  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimiser la </t>
+  </si>
+  <si>
+    <t>date de fin de projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en dispatchant les tâches </t>
+  </si>
+  <si>
+    <t>sur 2 machines différentes</t>
+  </si>
+  <si>
+    <t>Machines multiples</t>
+  </si>
+  <si>
+    <t>Légende :</t>
   </si>
 </sst>
 </file>
@@ -281,7 +308,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +369,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -511,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -552,6 +603,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -567,26 +632,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -891,6 +954,782 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="5.21875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="5" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1"/>
+    <col min="10" max="10" width="7.21875" style="22" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="F1" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3" s="16">
+        <v>1</v>
+      </c>
+      <c r="C3" s="37">
+        <v>9</v>
+      </c>
+      <c r="D3" s="34">
+        <v>32</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="30">
+        <v>2</v>
+      </c>
+      <c r="H3" s="40">
+        <f t="shared" ref="H3:H8" si="0">VLOOKUP($G3,$B$3:$C$8,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="I3" s="2">
+        <f>$H$3</f>
+        <v>7</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="11">
+        <f t="shared" ref="K3:K8" si="1">VLOOKUP($G3,$B$3:$D$8,3,FALSE)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="B4" s="16">
+        <v>2</v>
+      </c>
+      <c r="C4" s="37">
+        <v>7</v>
+      </c>
+      <c r="D4" s="34">
+        <v>29</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="31">
+        <v>3</v>
+      </c>
+      <c r="H4" s="37">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I4" s="5">
+        <f>SUM($H$3:$H4)</f>
+        <v>15</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="9">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5" s="16">
+        <v>3</v>
+      </c>
+      <c r="C5" s="37">
+        <v>8</v>
+      </c>
+      <c r="D5" s="34">
+        <v>22</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="32">
+        <v>1</v>
+      </c>
+      <c r="H5" s="38">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I5" s="8">
+        <f>SUM($H$3:$H5)</f>
+        <v>24</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="10">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="16">
+        <v>4</v>
+      </c>
+      <c r="C6" s="37">
+        <v>18</v>
+      </c>
+      <c r="D6" s="34">
+        <v>21</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="30">
+        <v>4</v>
+      </c>
+      <c r="H6" s="37">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="I6" s="5">
+        <f>H$6</f>
+        <v>18</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="9">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="16">
+        <v>5</v>
+      </c>
+      <c r="C7" s="37">
+        <v>9</v>
+      </c>
+      <c r="D7" s="34">
+        <v>37</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="31">
+        <v>6</v>
+      </c>
+      <c r="H7" s="37">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I7" s="5">
+        <f>SUM($H$6:$H7)</f>
+        <v>24</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="9">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="17">
+        <v>6</v>
+      </c>
+      <c r="C8" s="38">
+        <v>6</v>
+      </c>
+      <c r="D8" s="35">
+        <v>28</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="32">
+        <v>5</v>
+      </c>
+      <c r="H8" s="38">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I8" s="8">
+        <f>SUM($H$6:$H8)</f>
+        <v>33</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="10">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="28">
+        <f>MAX(I5,I8)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="62" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="33"/>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="J12"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="29"/>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="J13"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="36"/>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="22"/>
+      <c r="J14"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="39"/>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="J15"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="B16"/>
+      <c r="E16" s="22"/>
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:36">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17"/>
+      <c r="E17" s="22"/>
+      <c r="J17"/>
+    </row>
+    <row r="21" spans="1:36">
+      <c r="A21" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="4"/>
+      <c r="AG21" s="4"/>
+      <c r="AH21" s="4"/>
+      <c r="AI21" s="4"/>
+      <c r="AJ21" s="53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36">
+      <c r="A22" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="4"/>
+      <c r="AG22" s="4"/>
+      <c r="AH22" s="4"/>
+      <c r="AI22" s="4"/>
+      <c r="AJ22" s="56" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23" s="57"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="57"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="57"/>
+      <c r="P23" s="57"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="4"/>
+      <c r="AG23" s="4"/>
+      <c r="AH23" s="4"/>
+      <c r="AI23" s="4"/>
+      <c r="AJ23" s="53"/>
+    </row>
+    <row r="24" spans="1:36">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="R24" s="58"/>
+      <c r="S24" s="58"/>
+      <c r="T24" s="58"/>
+      <c r="U24" s="58"/>
+      <c r="V24" s="58"/>
+      <c r="W24" s="58"/>
+      <c r="X24" s="58"/>
+      <c r="Y24" s="58"/>
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="4"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="4"/>
+      <c r="AG24" s="4"/>
+      <c r="AH24" s="4"/>
+      <c r="AI24" s="4"/>
+      <c r="AJ24" s="53"/>
+    </row>
+    <row r="25" spans="1:36">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="4"/>
+      <c r="AF25" s="4"/>
+      <c r="AG25" s="4"/>
+      <c r="AH25" s="4"/>
+      <c r="AI25" s="4"/>
+      <c r="AJ25" s="53"/>
+    </row>
+    <row r="26" spans="1:36">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="4"/>
+      <c r="AF26" s="4"/>
+      <c r="AG26" s="4"/>
+      <c r="AH26" s="4"/>
+      <c r="AI26" s="4"/>
+      <c r="AJ26" s="53"/>
+    </row>
+    <row r="27" spans="1:36">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="4"/>
+      <c r="AF27" s="4"/>
+      <c r="AG27" s="4"/>
+      <c r="AH27" s="4"/>
+      <c r="AI27" s="4"/>
+      <c r="AJ27" s="53"/>
+    </row>
+    <row r="28" spans="1:36">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
+      <c r="AE28" s="4"/>
+      <c r="AF28" s="4"/>
+      <c r="AG28" s="4"/>
+      <c r="AH28" s="4"/>
+      <c r="AI28" s="4"/>
+      <c r="AJ28" s="53"/>
+    </row>
+    <row r="29" spans="1:36">
+      <c r="A29" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="59"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="59"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="59"/>
+      <c r="O29" s="59"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="59"/>
+      <c r="R29" s="59"/>
+      <c r="S29" s="59"/>
+      <c r="T29" s="59"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="4"/>
+      <c r="AF29" s="4"/>
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="4"/>
+      <c r="AI29" s="4"/>
+      <c r="AJ29" s="53"/>
+    </row>
+    <row r="30" spans="1:36">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="V30" s="60"/>
+      <c r="W30" s="60"/>
+      <c r="X30" s="60"/>
+      <c r="Y30" s="60"/>
+      <c r="Z30" s="60"/>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="4"/>
+      <c r="AE30" s="4"/>
+      <c r="AF30" s="4"/>
+      <c r="AG30" s="4"/>
+      <c r="AH30" s="4"/>
+      <c r="AI30" s="4"/>
+      <c r="AJ30" s="53"/>
+    </row>
+    <row r="31" spans="1:36">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB31" s="61"/>
+      <c r="AC31" s="61"/>
+      <c r="AD31" s="61"/>
+      <c r="AE31" s="61"/>
+      <c r="AF31" s="61"/>
+      <c r="AG31" s="61"/>
+      <c r="AH31" s="61"/>
+      <c r="AI31" s="61"/>
+      <c r="AJ31" s="53"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="F6:F8"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -926,7 +1765,7 @@
       </c>
       <c r="H2" s="24"/>
       <c r="I2" s="25" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="24"/>
@@ -958,7 +1797,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:14">
@@ -985,7 +1824,7 @@
         <v>Chicago</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:14">
@@ -1012,7 +1851,7 @@
         <v>1050</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:14">
@@ -1039,7 +1878,7 @@
         <v>1815</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:14" s="4" customFormat="1">
@@ -1070,7 +1909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R14"/>
   <sheetViews>
@@ -1724,371 +2563,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="2" max="2" width="5.21875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="7.21875" style="22" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:47">
-      <c r="A1" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="48" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47">
-      <c r="B2" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-    </row>
-    <row r="3" spans="1:47">
-      <c r="B3" s="16">
-        <v>1</v>
-      </c>
-      <c r="C3" s="42">
-        <v>9</v>
-      </c>
-      <c r="D3" s="39">
-        <v>32</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="35">
-        <v>2</v>
-      </c>
-      <c r="H3" s="45">
-        <f t="shared" ref="H3:H8" si="0">VLOOKUP($G3,$B$3:$C$8,2,FALSE)</f>
-        <v>7</v>
-      </c>
-      <c r="I3" s="2">
-        <f>$H$3</f>
-        <v>7</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="11">
-        <f t="shared" ref="K3:K8" si="1">VLOOKUP($G3,$B$3:$D$8,3,FALSE)</f>
-        <v>29</v>
-      </c>
-      <c r="V3" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
-      <c r="Y3" s="47"/>
-      <c r="Z3" s="47"/>
-      <c r="AA3" s="47"/>
-      <c r="AB3" s="47"/>
-    </row>
-    <row r="4" spans="1:47">
-      <c r="B4" s="16">
-        <v>2</v>
-      </c>
-      <c r="C4" s="42">
-        <v>7</v>
-      </c>
-      <c r="D4" s="39">
-        <v>29</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="36">
-        <v>3</v>
-      </c>
-      <c r="H4" s="42">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="I4" s="5">
-        <f>SUM($H$3:$H4)</f>
-        <v>15</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="9">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="AC4" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
-      <c r="AG4" s="34"/>
-      <c r="AH4" s="34"/>
-      <c r="AI4" s="34"/>
-      <c r="AJ4" s="34"/>
-      <c r="AK4" s="34"/>
-    </row>
-    <row r="5" spans="1:47">
-      <c r="B5" s="16">
-        <v>3</v>
-      </c>
-      <c r="C5" s="42">
-        <v>8</v>
-      </c>
-      <c r="D5" s="39">
-        <v>22</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="37">
-        <v>1</v>
-      </c>
-      <c r="H5" s="43">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I5" s="8">
-        <f>SUM($H$3:$H5)</f>
-        <v>24</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="10">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:47">
-      <c r="B6" s="16">
-        <v>4</v>
-      </c>
-      <c r="C6" s="42">
-        <v>18</v>
-      </c>
-      <c r="D6" s="39">
-        <v>21</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="35">
-        <v>4</v>
-      </c>
-      <c r="H6" s="42">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="I6" s="5">
-        <f>H$6</f>
-        <v>18</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="9">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:47">
-      <c r="B7" s="16">
-        <v>5</v>
-      </c>
-      <c r="C7" s="42">
-        <v>9</v>
-      </c>
-      <c r="D7" s="39">
-        <v>37</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="36">
-        <v>6</v>
-      </c>
-      <c r="H7" s="42">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I7" s="5">
-        <f>SUM($H$6:$H7)</f>
-        <v>24</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="9">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:47">
-      <c r="B8" s="17">
-        <v>6</v>
-      </c>
-      <c r="C8" s="43">
-        <v>6</v>
-      </c>
-      <c r="D8" s="40">
-        <v>28</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="37">
-        <v>5</v>
-      </c>
-      <c r="H8" s="43">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I8" s="8">
-        <f>SUM($H$6:$H8)</f>
-        <v>33</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="10">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:47">
-      <c r="F9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="33">
-        <f>MAX(I5,I8)</f>
-        <v>33</v>
-      </c>
-      <c r="M9" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="O9" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="49"/>
-      <c r="R9" s="49"/>
-      <c r="S9" s="49"/>
-      <c r="T9" s="49"/>
-      <c r="U9" s="49"/>
-      <c r="V9" s="49"/>
-      <c r="W9" s="49"/>
-      <c r="X9" s="49"/>
-      <c r="Y9" s="49"/>
-      <c r="Z9" s="49"/>
-      <c r="AA9" s="49"/>
-      <c r="AB9" s="49"/>
-      <c r="AC9" s="49"/>
-      <c r="AD9" s="49"/>
-      <c r="AE9" s="49"/>
-      <c r="AF9" s="49"/>
-    </row>
-    <row r="10" spans="1:47">
-      <c r="AG10" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH10" s="51"/>
-      <c r="AI10" s="51"/>
-      <c r="AJ10" s="51"/>
-      <c r="AK10" s="51"/>
-      <c r="AL10" s="51"/>
-    </row>
-    <row r="11" spans="1:47">
-      <c r="F11" s="38"/>
-      <c r="G11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM11" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN11" s="52"/>
-      <c r="AO11" s="52"/>
-      <c r="AP11" s="52"/>
-      <c r="AQ11" s="52"/>
-      <c r="AR11" s="52"/>
-      <c r="AS11" s="52"/>
-      <c r="AT11" s="52"/>
-      <c r="AU11" s="52"/>
-    </row>
-    <row r="12" spans="1:47">
-      <c r="F12" s="34"/>
-      <c r="G12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:47">
-      <c r="F13" s="41"/>
-      <c r="G13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:47">
-      <c r="F14" s="44"/>
-      <c r="G14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:47">
-      <c r="F16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="F6:F8"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>